<commit_message>
New changes, included calculate button
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13.42578125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="68" bestFit="1" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -429,7 +437,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Item Details</t>
+          <t>Delivery Time</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -450,88 +458,94 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>Delivery Person</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Order Details</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sneha pathak</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>mangoes</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Take Away</t>
+          <t>Delivery</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Paid</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Rajas</t>
+          <t>Not Paid</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rice: 1 | 
+Bhaji:   | 
+Bhakari:   | 
+Varan: 1 | 
+</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>rajas</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>bhakari</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>15.00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Delivery</t>
+          <t>Take Away</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Paid</t>
+          <t>Not Paid</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>Lomesh</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rice: 0 | 
+Bhaji:   | 
+Bhakari:   | 
+Varan: 0 | 
+</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>lomesh</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>asad</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>60</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -543,41 +557,194 @@
           <t>Not Paid</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Rajas</t>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rice: 1 | 
+Bhaji:   | 
+Bhakari:   | 
+Varan: 1 | 
+</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>sds</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>110</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Not Paid</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rice: 1 | 
+Bhaji: 1  | 
+Bhakari: 3  | 
+Varan: 2 | 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>80</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Not Paid</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rice: 0 | 
+Bhaji: 1  | 
+Bhakari: 3  | 
+Varan: 1 | 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>60</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Not Paid</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rice: 0 | 
+Bhaji: 1  | 
+Bhakari: 3  | 
+Varan: 0 | 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>60</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Not Paid</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rice: 0 | 
+Bhaji: 1special  | 
+Bhakari: 3matar paneer  | 
+Varan: 0 | 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>60</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Not Paid</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Rajas</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rice: 1 | 
+Bhaji: 1 matar  | 
+Bhakari: 1 bhendi  | 
+Varan: 1 | 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>60</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>Delivery</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Paid</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Rajas</t>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Not Paid</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rice: 1 | 
+Bhaji: 1   | 
+Bhakari: 1   | 
+Varan: 1 | 
+</t>
         </is>
       </c>
     </row>

</xml_diff>